<commit_message>
Fixed XLSX Report Generation
</commit_message>
<xml_diff>
--- a/backend/public/dog_details.xlsx
+++ b/backend/public/dog_details.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Dog Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Catcher Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Dogs Report" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -398,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,90 +415,413 @@
       <c r="D1" t="str">
         <v>Description</v>
       </c>
+      <c r="E1" t="str">
+        <v>Catcher ID</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Catcher's Name</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Catcher's Contact Number</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Catching Location</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Catching Location Details</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Releasing Location</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Catched At</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Spot Photo</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Vet ID</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Vet's Name</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Vet's Contact Number</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Surgery date</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Surgery Photo</v>
+      </c>
+      <c r="R1" t="str">
+        <v>dogWeight</v>
+      </c>
+      <c r="S1" t="str">
+        <v>observations</v>
+      </c>
+      <c r="T1" t="str">
+        <v>temperature</v>
+      </c>
+      <c r="U1" t="str">
+        <v>atropine</v>
+      </c>
+      <c r="V1" t="str">
+        <v>dexa</v>
+      </c>
+      <c r="W1" t="str">
+        <v>dicrysticin</v>
+      </c>
+      <c r="X1" t="str">
+        <v>earNotched</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>enrodac</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>ketamin</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>melonex</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>prednisolone</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>procedure</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>stadren</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>xylazine</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Caretaker ID</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Caretaker's Name</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Caretaker's Contact Number</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>Day 1 Report ID</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>Day 1 Food Intake</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>Day 1 Water Intake</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>Day 1 Antibiotics</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>Day 1 Painkiller</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>Day 1 Photo</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>surgeryNotesPhoto</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>Day 2 Report ID</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>Day 2 Food Intake</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>Day 2 Water Intake</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>Day 2 Antibiotics</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>Day 2 Painkiller</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>Day 2 Photo</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>6563199b47985803bf7d7e20</v>
+        <v>654d0f017a0b20ccc6394e18</v>
       </c>
       <c r="B2" t="str">
-        <v>WH</v>
+        <v>BL</v>
       </c>
       <c r="C2" t="str">
         <v>male</v>
       </c>
       <c r="D2" t="str">
-        <v>Najan</v>
+        <v xml:space="preserve">kuch toh timepass </v>
+      </c>
+      <c r="E2" t="str">
+        <v>653fe853df4866ef5e596994</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Rohit Sharma</v>
+      </c>
+      <c r="G2" t="str">
+        <v>9321781063</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Lat :12, Long: 15</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Somewhere near the park</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Thu Nov 09 2023 22:25:29 GMT+0530 (India Standard Time)</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Click to open photo</v>
+      </c>
+      <c r="M2" t="str">
+        <v>65476fac7e7f9657d213a5a5</v>
+      </c>
+      <c r="N2" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="O2" t="str">
+        <v>9321781064</v>
+      </c>
+      <c r="P2" t="str">
+        <v>Sat Nov 11 2023 00:00:00 GMT+0530 (India Standard Time)</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>Click to open photo</v>
+      </c>
+      <c r="R2">
+        <v>123123</v>
+      </c>
+      <c r="S2" t="str">
+        <v>idk somthing</v>
+      </c>
+      <c r="T2">
+        <v>23</v>
+      </c>
+      <c r="U2" t="str">
+        <v>324ml</v>
+      </c>
+      <c r="V2" t="str">
+        <v>34ml</v>
+      </c>
+      <c r="W2" t="str">
+        <v>45ml</v>
+      </c>
+      <c r="X2" t="str">
+        <v>ha</v>
+      </c>
+      <c r="Y2" t="str">
+        <v>321ml</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>123ml</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>34ml</v>
+      </c>
+      <c r="AB2" t="str">
+        <v>32ml</v>
+      </c>
+      <c r="AC2" t="str">
+        <v>kuch toh</v>
+      </c>
+      <c r="AD2" t="str">
+        <v>56ml</v>
+      </c>
+      <c r="AE2" t="str">
+        <v>2ml</v>
+      </c>
+      <c r="AF2" t="str">
+        <v>65476fac7e7f9657d213a5a5</v>
+      </c>
+      <c r="AG2" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="AH2" t="str">
+        <v>9321781064</v>
+      </c>
+      <c r="AI2" t="str">
+        <v>654f91e8a0bccb86644f9523</v>
+      </c>
+      <c r="AJ2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AK2" t="str">
+        <v>no</v>
+      </c>
+      <c r="AL2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AM2" t="str">
+        <v>no</v>
+      </c>
+      <c r="AN2" t="str">
+        <v>Click to open photo</v>
+      </c>
+      <c r="AO2" t="str">
+        <v>Sat Nov 11 2023 00:00:00 GMT+0530 (India Standard Time)</v>
       </c>
     </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Catcher ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Contact Number</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Catching Location</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Catching Location Details</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Releasing Location</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Catched At</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Spot Photo</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
+    <row r="3">
+      <c r="A3" t="str">
+        <v>65524c2d4d0dc30557f619c7</v>
+      </c>
+      <c r="B3" t="str">
+        <v>TM</v>
+      </c>
+      <c r="C3" t="str">
+        <v>male</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Kuch toh about dog</v>
+      </c>
+      <c r="E3" t="str">
         <v>653fe853df4866ef5e596994</v>
       </c>
-      <c r="B2" t="str">
+      <c r="F3" t="str">
         <v>Rohit Sharma</v>
       </c>
-      <c r="C2" t="str">
+      <c r="G3" t="str">
         <v>9321781063</v>
       </c>
-      <c r="D2" t="str">
-        <v>Kuch toh naya</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Yup naya</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Sun Nov 26 2023 15:40:35 GMT+0530 (India Standard Time)</v>
-      </c>
-      <c r="H2" t="str">
+      <c r="H3" t="str">
+        <v>Kuch toh</v>
+      </c>
+      <c r="I3" t="str">
+        <v xml:space="preserve">Idk smthn. </v>
+      </c>
+      <c r="K3" t="str">
+        <v>Mon Nov 13 2023 21:47:49 GMT+0530 (India Standard Time)</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Click to open photo</v>
+      </c>
+      <c r="M3" t="str">
+        <v>654d194d3e52b6d1ebd6e4c7</v>
+      </c>
+      <c r="N3" t="str">
+        <v>ryan doe</v>
+      </c>
+      <c r="O3" t="str">
+        <v>8850596131</v>
+      </c>
+      <c r="P3" t="str">
+        <v>Mon Nov 13 2023 00:00:00 GMT+0530 (India Standard Time)</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>Click to open photo</v>
+      </c>
+      <c r="R3">
+        <v>15</v>
+      </c>
+      <c r="S3" t="str">
+        <v>Looks good, he's a good boy</v>
+      </c>
+      <c r="T3">
+        <v>73</v>
+      </c>
+      <c r="U3" t="str">
+        <v>02ml</v>
+      </c>
+      <c r="V3" t="str">
+        <v>23ml</v>
+      </c>
+      <c r="W3" t="str">
+        <v>1ml</v>
+      </c>
+      <c r="X3" t="str">
+        <v>Yea</v>
+      </c>
+      <c r="Y3" t="str">
+        <v>72ml</v>
+      </c>
+      <c r="Z3" t="str">
+        <v>12ml</v>
+      </c>
+      <c r="AA3" t="str">
+        <v>22ml</v>
+      </c>
+      <c r="AB3" t="str">
+        <v>62ml</v>
+      </c>
+      <c r="AC3" t="str">
+        <v>Idk</v>
+      </c>
+      <c r="AD3" t="str">
+        <v>81ml</v>
+      </c>
+      <c r="AE3" t="str">
+        <v>15ml</v>
+      </c>
+      <c r="AF3" t="str">
+        <v>65524b4d040afd205348b14d</v>
+      </c>
+      <c r="AG3" t="str">
+        <v>Virat Kohli</v>
+      </c>
+      <c r="AH3" t="str">
+        <v>9819916102</v>
+      </c>
+      <c r="AI3" t="str">
+        <v>65524fe966fcd9fd11012c9f</v>
+      </c>
+      <c r="AJ3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AK3" t="str">
+        <v>no</v>
+      </c>
+      <c r="AL3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AM3" t="str">
+        <v>no</v>
+      </c>
+      <c r="AN3" t="str">
+        <v>Click to open photo</v>
+      </c>
+      <c r="AO3" t="str">
+        <v>Mon Nov 13 2023 00:00:00 GMT+0530 (India Standard Time)</v>
+      </c>
+      <c r="AQ3" t="str">
+        <v>6552501c66fcd9fd11012cb0</v>
+      </c>
+      <c r="AR3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AS3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AT3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AU3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AV3" t="str">
         <v>Click to open photo</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
+    <hyperlink ref="AN2" r:id="rId3"/>
+    <hyperlink ref="L3" r:id="rId4"/>
+    <hyperlink ref="Q3" r:id="rId5"/>
+    <hyperlink ref="AN3" r:id="rId6"/>
+    <hyperlink ref="AV3" r:id="rId7"/>
   </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AV3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated backend report fix
</commit_message>
<xml_diff>
--- a/backend/public/dog_details.xlsx
+++ b/backend/public/dog_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,108 +464,99 @@
         <v>observations</v>
       </c>
       <c r="U1" t="str">
+        <v>surgeryNotesPhoto</v>
+      </c>
+      <c r="V1" t="str">
         <v>atropine</v>
       </c>
-      <c r="V1" t="str">
+      <c r="W1" t="str">
         <v>dexa</v>
       </c>
-      <c r="W1" t="str">
+      <c r="X1" t="str">
         <v>dicrysticin</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Y1" t="str">
         <v>earNotched</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="Z1" t="str">
         <v>enrodac</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AA1" t="str">
         <v>ketamin</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AB1" t="str">
         <v>melonex</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AC1" t="str">
         <v>prednisolone</v>
       </c>
-      <c r="AC1" t="str">
+      <c r="AD1" t="str">
         <v>procedure</v>
       </c>
-      <c r="AD1" t="str">
+      <c r="AE1" t="str">
         <v>stadren</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="AF1" t="str">
         <v>xylazine</v>
       </c>
-      <c r="AF1" t="str">
+      <c r="AG1" t="str">
         <v>Caretaker ID</v>
       </c>
-      <c r="AG1" t="str">
+      <c r="AH1" t="str">
         <v>Caretaker's Name</v>
       </c>
-      <c r="AH1" t="str">
+      <c r="AI1" t="str">
         <v>Caretaker's Contact Number</v>
       </c>
-      <c r="AI1" t="str">
+      <c r="AJ1" t="str">
         <v>Day 1 Report ID</v>
       </c>
-      <c r="AJ1" t="str">
+      <c r="AK1" t="str">
         <v>Day 1 Food Intake</v>
       </c>
-      <c r="AK1" t="str">
+      <c r="AL1" t="str">
         <v>Day 1 Water Intake</v>
       </c>
-      <c r="AL1" t="str">
+      <c r="AM1" t="str">
+        <v>Day 1 Stool</v>
+      </c>
+      <c r="AN1" t="str">
         <v>Day 1 Antibiotics</v>
       </c>
-      <c r="AM1" t="str">
+      <c r="AO1" t="str">
         <v>Day 1 Painkiller</v>
       </c>
-      <c r="AN1" t="str">
+      <c r="AP1" t="str">
         <v>Day 1 Photo</v>
       </c>
-      <c r="AO1" t="str">
+      <c r="AQ1" t="str">
         <v>Date</v>
       </c>
-      <c r="AP1" t="str">
+      <c r="AR1" t="str">
         <v>Day 2 Report ID</v>
       </c>
-      <c r="AQ1" t="str">
+      <c r="AS1" t="str">
         <v>Day 2 Food Intake</v>
       </c>
-      <c r="AR1" t="str">
+      <c r="AT1" t="str">
         <v>Day 2 Water Intake</v>
       </c>
-      <c r="AS1" t="str">
+      <c r="AU1" t="str">
+        <v>Day 2 Stool</v>
+      </c>
+      <c r="AV1" t="str">
         <v>Day 2 Antibiotics</v>
       </c>
-      <c r="AT1" t="str">
+      <c r="AW1" t="str">
         <v>Day 2 Painkiller</v>
       </c>
-      <c r="AU1" t="str">
+      <c r="AX1" t="str">
         <v>Day 2 Photo</v>
-      </c>
-      <c r="AV1" t="str">
-        <v>Day 3 Report ID</v>
-      </c>
-      <c r="AW1" t="str">
-        <v>Day 3 Food Intake</v>
-      </c>
-      <c r="AX1" t="str">
-        <v>Day 3 Water Intake</v>
-      </c>
-      <c r="AY1" t="str">
-        <v>Day 3 Antibiotics</v>
-      </c>
-      <c r="AZ1" t="str">
-        <v>Day 3 Painkiller</v>
-      </c>
-      <c r="BA1" t="str">
-        <v>Day 3 Photo</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>656cd7787e4d22a03b6a073c</v>
+        <v>65b8fd6eefc71c45b4e1adbd</v>
       </c>
       <c r="B2" t="str">
         <v>Dark Brown</v>
@@ -574,163 +565,147 @@
         <v>male</v>
       </c>
       <c r="D2" t="str">
-        <v>Good boy</v>
+        <v>Nice dog</v>
       </c>
       <c r="E2" t="str">
-        <v>656c4711638b32e06dd60de1</v>
+        <v>6572f8f05bf1a8dd5eb6d3de</v>
       </c>
       <c r="F2" t="str">
-        <v>John Doe</v>
+        <v>Manoj Oswal</v>
       </c>
       <c r="G2" t="str">
-        <v>9321781063</v>
+        <v>9890044455</v>
       </c>
       <c r="H2" t="str">
-        <v>Morya avenue, chogale nagar, 6VQ9+5FX, Kajupada, Borivali, Mumbai, Maharashtra 400066, India</v>
+        <v>BMC KUJU PADA NAGARI AROGYA KENDRA, MORYA AVENUE, Sant Gadge Maharaj Marg, काजुपाडा, बोरिवली ईस्ट, मुंबई, महाराष्ट्र 400060, India</v>
       </c>
       <c r="I2" t="str">
-        <v>Near the park</v>
+        <v>Near my house</v>
       </c>
       <c r="K2" t="str">
-        <v>Mon Dec 04 2023 01:01:04 GMT+0530 (India Standard Time)</v>
+        <v>Tue Jan 30 2024 19:15:18 GMT+0530 (India Standard Time)</v>
       </c>
       <c r="L2" t="str">
-        <v>Click to open photo</v>
+        <v>spotPhoto-1706622318257.jpeg</v>
       </c>
       <c r="M2" t="str">
-        <v>656c4711638b32e06dd60de1</v>
+        <v>6572f8f05bf1a8dd5eb6d3de</v>
       </c>
       <c r="N2" t="str">
-        <v>John Doe</v>
+        <v>Manoj Oswal</v>
       </c>
       <c r="O2" t="str">
-        <v>9321781063</v>
+        <v>9890044455</v>
       </c>
       <c r="P2" t="str">
-        <v>Mon Dec 04 2023 00:00:00 GMT+0530 (India Standard Time)</v>
+        <v>Sat Jan 27 2024 00:00:00 GMT+0530 (India Standard Time)</v>
       </c>
       <c r="Q2" t="str">
-        <v>Click to open photo</v>
+        <v>surgeryPhoto-1706622636849.jpeg</v>
       </c>
       <c r="R2">
         <v>15</v>
       </c>
       <c r="S2">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="T2" t="str">
-        <v>Hsj</v>
+        <v xml:space="preserve">Nice </v>
       </c>
       <c r="U2" t="str">
-        <v>Wa</v>
+        <v>uploads/surgeryNotesPhoto-1706622582405.jpeg</v>
       </c>
       <c r="V2" t="str">
-        <v>Js</v>
+        <v>S</v>
       </c>
       <c r="W2" t="str">
-        <v>A</v>
+        <v>1</v>
       </c>
       <c r="X2" t="str">
-        <v>Ye</v>
+        <v>I</v>
       </c>
       <c r="Y2" t="str">
-        <v>A</v>
+        <v xml:space="preserve">Yes </v>
       </c>
       <c r="Z2" t="str">
-        <v>A</v>
+        <v>S</v>
       </c>
       <c r="AA2" t="str">
-        <v>Ja</v>
+        <v>I</v>
       </c>
       <c r="AB2" t="str">
-        <v>A</v>
+        <v>S</v>
       </c>
       <c r="AC2" t="str">
         <v>S</v>
       </c>
       <c r="AD2" t="str">
-        <v>Sd</v>
+        <v xml:space="preserve">Within </v>
       </c>
       <c r="AE2" t="str">
-        <v>Js</v>
+        <v>I</v>
       </c>
       <c r="AF2" t="str">
-        <v>656c4711638b32e06dd60de1</v>
+        <v>15ml</v>
       </c>
       <c r="AG2" t="str">
-        <v>John Doe</v>
+        <v>6572f8f05bf1a8dd5eb6d3de</v>
       </c>
       <c r="AH2" t="str">
-        <v>9321781063</v>
+        <v>Manoj Oswal</v>
       </c>
       <c r="AI2" t="str">
-        <v>656cd8627e4d22a03b6a0774</v>
+        <v>9890044455</v>
       </c>
       <c r="AJ2" t="str">
-        <v>yes</v>
+        <v>65b90465c85e4ace9259d778</v>
       </c>
       <c r="AK2" t="str">
         <v>no</v>
       </c>
       <c r="AL2" t="str">
+        <v>yes</v>
+      </c>
+      <c r="AN2" t="str">
         <v>no</v>
       </c>
-      <c r="AM2" t="str">
+      <c r="AO2" t="str">
         <v>yes</v>
       </c>
-      <c r="AN2" t="str">
-        <v>Click to open photo</v>
-      </c>
-      <c r="AO2" t="str">
-        <v>Mon Dec 04 2023 00:00:00 GMT+0530 (India Standard Time)</v>
-      </c>
       <c r="AP2" t="str">
-        <v>656cd87a7e4d22a03b6a0786</v>
+        <v>uploads\photo-1706624100910.png</v>
       </c>
       <c r="AQ2" t="str">
-        <v>yes</v>
+        <v>Tue Jan 30 2024 00:00:00 GMT+0530 (India Standard Time)</v>
       </c>
       <c r="AR2" t="str">
-        <v>yes</v>
+        <v>65b90606c85e4ace9259d7a1</v>
       </c>
       <c r="AS2" t="str">
         <v>yes</v>
       </c>
       <c r="AT2" t="str">
+        <v>no</v>
+      </c>
+      <c r="AV2" t="str">
         <v>yes</v>
       </c>
-      <c r="AU2" t="str">
-        <v>Click to open photo</v>
-      </c>
-      <c r="AV2" t="str">
-        <v>656cdc908f252f7108b49191</v>
-      </c>
       <c r="AW2" t="str">
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="AX2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="AY2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="AZ2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="BA2" t="str">
-        <v>Click to open photo</v>
+        <v>uploads\photo-1706624518423.png</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
     <hyperlink ref="Q2" r:id="rId2"/>
-    <hyperlink ref="AN2" r:id="rId3"/>
-    <hyperlink ref="AU2" r:id="rId4"/>
-    <hyperlink ref="BA2" r:id="rId5"/>
+    <hyperlink ref="AP2" r:id="rId3"/>
+    <hyperlink ref="AX2" r:id="rId4"/>
   </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BA2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AX2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>